<commit_message>
Updated index.html and excel
</commit_message>
<xml_diff>
--- a/Review papers.xlsx
+++ b/Review papers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n216_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099D4ED6-DB47-41DF-99DA-A221B1CB153E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141FE8AB-C932-43A8-AD37-9100C638CC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GANs" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="237">
   <si>
     <t>Title</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Ahmed M. Alaa, Boris van Breugel, Evgeny Saveliev, Mihaela van der Schaar</t>
   </si>
   <si>
-    <t>Model assessment</t>
-  </si>
-  <si>
     <t>SIVEP-Gripe COVID-19 patient data
 MNIST data
  AmsterdamUMCdb data</t>
@@ -797,9 +794,6 @@
     <t>2021/11/01</t>
   </si>
   <si>
-    <t>1900/01/00</t>
-  </si>
-  <si>
     <t>2021/11/16</t>
   </si>
   <si>
@@ -864,17 +858,20 @@
   </si>
   <si>
     <t>2022/06/26</t>
+  </si>
+  <si>
+    <t>2019/08/01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -882,7 +879,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -890,14 +887,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -905,13 +902,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -938,7 +935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -963,10 +960,13 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1246,30 +1246,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA087E-C0D3-469D-A8E2-9DE3389B497D}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="3"/>
-    <col min="2" max="2" width="145.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="141.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.25" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="145.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="141.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="40" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="88.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="72.4140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="7"/>
+    <col min="11" max="11" width="88.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1278,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1305,7 +1305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="93" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="110.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
@@ -1340,7 +1340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="3" customFormat="1" ht="78.75">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>21</v>
@@ -1378,7 +1378,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="63">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>29</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>30</v>
@@ -1413,10 +1413,10 @@
         <v>34</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="108.5" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="110.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1426,8 +1426,8 @@
       <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>215</v>
+      <c r="D5" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>37</v>
@@ -1451,7 +1451,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="77.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="78.75">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>45</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>46</v>
@@ -1489,7 +1489,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="47.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>54</v>
@@ -1524,7 +1524,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="31.5">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>60</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>61</v>
@@ -1559,7 +1559,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="3" customFormat="1">
       <c r="B9" s="3" t="s">
         <v>67</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>69</v>
@@ -1591,7 +1591,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="47.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>76</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>77</v>
@@ -1623,7 +1623,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="31.5">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>83</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>38</v>
@@ -1652,7 +1652,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="62" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="63">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>89</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>90</v>
@@ -1690,7 +1690,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="62" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="63">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>98</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>99</v>
@@ -1728,7 +1728,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="47.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -1739,71 +1739,71 @@
         <v>106</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:12" ht="63">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="62" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L15" s="6" t="s">
+    </row>
+    <row r="16" spans="1:12" ht="47.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>13</v>
@@ -1812,129 +1812,129 @@
         <v>62</v>
       </c>
       <c r="I16" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="L16" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="L16" s="5" t="s">
+    </row>
+    <row r="17" spans="1:12" ht="78.75">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="J17" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K17" s="5" t="s">
+    </row>
+    <row r="18" spans="1:12" ht="63">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="62" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="K18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:12" ht="63">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="62" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="K19" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K19" s="6" t="s">
+    </row>
+    <row r="20" spans="1:12" ht="94.5">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>37</v>
@@ -1949,30 +1949,30 @@
         <v>40</v>
       </c>
       <c r="I20" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="K20" s="6" t="s">
+    </row>
+    <row r="21" spans="1:12" ht="63">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="62" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
-        <v>1</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>13</v>
@@ -1981,30 +1981,30 @@
         <v>40</v>
       </c>
       <c r="I21" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="K21" s="6" t="s">
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>13</v>
@@ -2013,30 +2013,30 @@
         <v>23</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="6" t="s">
+    </row>
+    <row r="23" spans="1:12" ht="94.5">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="93" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>13</v>
@@ -2045,30 +2045,30 @@
         <v>23</v>
       </c>
       <c r="I23" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="K23" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K23" s="5" t="s">
+    </row>
+    <row r="24" spans="1:12" ht="47.25">
+      <c r="A24" s="3">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>13</v>
@@ -2077,62 +2077,62 @@
         <v>23</v>
       </c>
       <c r="I24" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="K24" s="5" t="s">
+    </row>
+    <row r="25" spans="1:12" ht="78.75">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="J25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="K25" s="5" t="s">
+    </row>
+    <row r="26" spans="1:12" ht="47.25">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
-        <v>1</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>13</v>
@@ -2141,33 +2141,33 @@
         <v>23</v>
       </c>
       <c r="I26" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="K26" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="L26" s="5" t="s">
+    </row>
+    <row r="27" spans="1:12" ht="78.75">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
-        <v>1</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>13</v>
@@ -2176,83 +2176,83 @@
         <v>23</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K27" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="63">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="62" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="K28" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="L28" s="5" t="s">
+    </row>
+    <row r="29" spans="1:12" ht="63">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="62" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I29" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="K29" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="L29" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:12">
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="5"/>
@@ -2312,7 +2312,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>